<commit_message>
feat: read from args
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -8,8 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mental/Desktop/project/excel2jira/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1117AE-AE65-D345-8F8D-1A81F79C92C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="15940"/>
+    <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,22 +46,22 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>test</t>
+    <t>jira_id</t>
+  </si>
+  <si>
+    <t>sample: jira_id exists</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>jira_id</t>
+    <t>sample: project not exists</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>failed.\ncan't find project named test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -74,6 +75,15 @@
       <name val="等线"/>
       <family val="4"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -98,16 +108,19 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -416,44 +429,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="29" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>11</v>
       </c>
       <c r="C2">
-        <v>111</v>
-      </c>
-      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
         <v>5</v>
+      </c>
+      <c r="B3">
+        <v>22</v>
+      </c>
+      <c r="C3">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add support field: priority
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mental/Desktop/project/excel2jira/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1117AE-AE65-D345-8F8D-1A81F79C92C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F555209-9E41-A842-AF71-A0CA43A6CF7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>project</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -49,11 +49,22 @@
     <t>jira_id</t>
   </si>
   <si>
+    <t>sample: project not exists</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>priority</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>sample: jira_id exists</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sample: project not exists</t>
+  </si>
+  <si>
+    <t>high</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TSET-1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -429,7 +440,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -438,7 +449,7 @@
     <col min="1" max="1" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -449,12 +460,15 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>11</v>
@@ -462,13 +476,16 @@
       <c r="C2">
         <v>11</v>
       </c>
-      <c r="D2">
-        <v>11</v>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>22</v>

</xml_diff>